<commit_message>
Editing Workload distribution file
Replaced Message Chains task with Long Method (counting statements) for Andrii
</commit_message>
<xml_diff>
--- a/Workload distribution.xlsx
+++ b/Workload distribution.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F67C31-D035-4621-95B0-7656C1A797F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,9 +25,6 @@
     <t>Long Parameter List</t>
   </si>
   <si>
-    <t>Message Chains</t>
-  </si>
-  <si>
     <t>Points</t>
   </si>
   <si>
@@ -52,12 +50,15 @@
   </si>
   <si>
     <t>Andrii</t>
+  </si>
+  <si>
+    <t>Long Method (counting statements)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -376,11 +377,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -400,24 +401,24 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -440,25 +441,25 @@
     </row>
     <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding Temporary Field Smell Detector + some minor changes to the structure (for easier execution)
</commit_message>
<xml_diff>
--- a/Workload distribution.xlsx
+++ b/Workload distribution.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F67C31-D035-4621-95B0-7656C1A797F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +57,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -377,7 +376,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
@@ -388,7 +387,7 @@
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
     <col min="2" max="2" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="40.109375" bestFit="1" customWidth="1"/>

</xml_diff>